<commit_message>
Final Figures and Tables
</commit_message>
<xml_diff>
--- a/manuscript/tables/Table-S5a-GO-pval-0.05-DE.xlsx
+++ b/manuscript/tables/Table-S5a-GO-pval-0.05-DE.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table-S3a-GO-pval-0.05-DE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Table-S5a-GO-pval-0.05-DE" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -7548,11 +7548,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7568,6 +7569,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7612,8 +7620,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7641,59 +7653,59 @@
   <dimension ref="A1:L875"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.57142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="122.591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="310.724489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="121.224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="307.377551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7713,7 +7725,7 @@
       <c r="E2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -7751,7 +7763,7 @@
       <c r="E3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -7789,7 +7801,7 @@
       <c r="E4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -7827,7 +7839,7 @@
       <c r="E5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -7865,7 +7877,7 @@
       <c r="E6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -7903,7 +7915,7 @@
       <c r="E7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -7941,7 +7953,7 @@
       <c r="E8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -7979,7 +7991,7 @@
       <c r="E9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -8017,7 +8029,7 @@
       <c r="E10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -8055,7 +8067,7 @@
       <c r="E11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -8093,7 +8105,7 @@
       <c r="E12" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -8131,7 +8143,7 @@
       <c r="E13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="0" t="s">
@@ -8169,7 +8181,7 @@
       <c r="E14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -8207,7 +8219,7 @@
       <c r="E15" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="0" t="s">
@@ -8245,7 +8257,7 @@
       <c r="E16" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -8283,7 +8295,7 @@
       <c r="E17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -8321,7 +8333,7 @@
       <c r="E18" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="0" t="s">
@@ -8359,7 +8371,7 @@
       <c r="E19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="0" t="s">
@@ -8397,7 +8409,7 @@
       <c r="E20" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="0" t="s">
@@ -8435,7 +8447,7 @@
       <c r="E21" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G21" s="0" t="s">
@@ -8473,7 +8485,7 @@
       <c r="E22" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G22" s="0" t="s">
@@ -8511,7 +8523,7 @@
       <c r="E23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G23" s="0" t="s">
@@ -8549,7 +8561,7 @@
       <c r="E24" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G24" s="0" t="s">
@@ -8587,7 +8599,7 @@
       <c r="E25" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G25" s="0" t="s">
@@ -8625,7 +8637,7 @@
       <c r="E26" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G26" s="0" t="s">
@@ -8663,7 +8675,7 @@
       <c r="E27" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G27" s="0" t="s">
@@ -8701,7 +8713,7 @@
       <c r="E28" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G28" s="0" t="s">
@@ -8739,7 +8751,7 @@
       <c r="E29" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G29" s="0" t="s">
@@ -8777,7 +8789,7 @@
       <c r="E30" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G30" s="0" t="s">
@@ -8815,7 +8827,7 @@
       <c r="E31" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G31" s="0" t="s">
@@ -8853,7 +8865,7 @@
       <c r="E32" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G32" s="0" t="s">
@@ -8891,7 +8903,7 @@
       <c r="E33" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="0" t="s">
@@ -8929,7 +8941,7 @@
       <c r="E34" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G34" s="0" t="s">
@@ -8967,7 +8979,7 @@
       <c r="E35" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="0" t="s">
@@ -9005,7 +9017,7 @@
       <c r="E36" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G36" s="0" t="s">
@@ -9043,7 +9055,7 @@
       <c r="E37" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="0" t="s">
@@ -9081,7 +9093,7 @@
       <c r="E38" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G38" s="0" t="s">
@@ -9119,7 +9131,7 @@
       <c r="E39" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G39" s="0" t="s">
@@ -9157,7 +9169,7 @@
       <c r="E40" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G40" s="0" t="s">
@@ -9195,7 +9207,7 @@
       <c r="E41" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G41" s="0" t="s">
@@ -9233,7 +9245,7 @@
       <c r="E42" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G42" s="0" t="s">
@@ -9271,7 +9283,7 @@
       <c r="E43" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G43" s="0" t="s">
@@ -9309,7 +9321,7 @@
       <c r="E44" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G44" s="0" t="s">
@@ -9347,7 +9359,7 @@
       <c r="E45" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G45" s="0" t="s">
@@ -9385,7 +9397,7 @@
       <c r="E46" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G46" s="0" t="s">
@@ -9423,7 +9435,7 @@
       <c r="E47" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G47" s="0" t="s">
@@ -9461,7 +9473,7 @@
       <c r="E48" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G48" s="0" t="s">
@@ -9499,7 +9511,7 @@
       <c r="E49" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G49" s="0" t="s">
@@ -9537,7 +9549,7 @@
       <c r="E50" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G50" s="0" t="s">
@@ -9575,7 +9587,7 @@
       <c r="E51" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G51" s="0" t="s">
@@ -9613,7 +9625,7 @@
       <c r="E52" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G52" s="0" t="s">
@@ -9651,7 +9663,7 @@
       <c r="E53" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G53" s="0" t="s">
@@ -9689,7 +9701,7 @@
       <c r="E54" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="0" t="s">
@@ -9727,7 +9739,7 @@
       <c r="E55" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G55" s="0" t="s">
@@ -9765,7 +9777,7 @@
       <c r="E56" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G56" s="0" t="s">
@@ -9803,7 +9815,7 @@
       <c r="E57" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G57" s="0" t="s">
@@ -9841,7 +9853,7 @@
       <c r="E58" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G58" s="0" t="s">
@@ -9879,7 +9891,7 @@
       <c r="E59" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G59" s="0" t="s">
@@ -9917,7 +9929,7 @@
       <c r="E60" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G60" s="0" t="s">
@@ -9955,7 +9967,7 @@
       <c r="E61" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G61" s="0" t="s">
@@ -9993,7 +10005,7 @@
       <c r="E62" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="0" t="s">
@@ -10031,7 +10043,7 @@
       <c r="E63" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G63" s="0" t="s">
@@ -10069,7 +10081,7 @@
       <c r="E64" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G64" s="0" t="s">
@@ -10107,7 +10119,7 @@
       <c r="E65" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G65" s="0" t="s">
@@ -10145,7 +10157,7 @@
       <c r="E66" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G66" s="0" t="s">
@@ -10183,7 +10195,7 @@
       <c r="E67" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F67" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G67" s="0" t="s">
@@ -10221,7 +10233,7 @@
       <c r="E68" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G68" s="0" t="s">
@@ -10259,7 +10271,7 @@
       <c r="E69" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G69" s="0" t="s">
@@ -10297,7 +10309,7 @@
       <c r="E70" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G70" s="0" t="s">
@@ -10335,7 +10347,7 @@
       <c r="E71" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G71" s="0" t="s">
@@ -10373,7 +10385,7 @@
       <c r="E72" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G72" s="0" t="s">
@@ -10411,7 +10423,7 @@
       <c r="E73" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G73" s="0" t="s">
@@ -10449,7 +10461,7 @@
       <c r="E74" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G74" s="0" t="s">
@@ -10487,7 +10499,7 @@
       <c r="E75" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F75" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G75" s="0" t="s">
@@ -10525,7 +10537,7 @@
       <c r="E76" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F76" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G76" s="0" t="s">
@@ -10563,7 +10575,7 @@
       <c r="E77" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G77" s="0" t="s">
@@ -10601,7 +10613,7 @@
       <c r="E78" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G78" s="0" t="s">
@@ -10639,7 +10651,7 @@
       <c r="E79" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G79" s="0" t="s">
@@ -10677,7 +10689,7 @@
       <c r="E80" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F80" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G80" s="0" t="s">
@@ -10715,7 +10727,7 @@
       <c r="E81" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F81" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G81" s="0" t="s">
@@ -10753,7 +10765,7 @@
       <c r="E82" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G82" s="0" t="s">
@@ -10791,7 +10803,7 @@
       <c r="E83" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G83" s="0" t="s">
@@ -10829,7 +10841,7 @@
       <c r="E84" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F84" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G84" s="0" t="s">
@@ -10867,7 +10879,7 @@
       <c r="E85" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="F85" s="1" t="s">
+      <c r="F85" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G85" s="0" t="s">
@@ -10905,7 +10917,7 @@
       <c r="E86" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="F86" s="1" t="s">
+      <c r="F86" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G86" s="0" t="s">
@@ -10943,7 +10955,7 @@
       <c r="E87" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="F87" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G87" s="0" t="s">
@@ -10981,7 +10993,7 @@
       <c r="E88" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F88" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G88" s="0" t="s">
@@ -11019,7 +11031,7 @@
       <c r="E89" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F89" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G89" s="0" t="s">
@@ -11057,7 +11069,7 @@
       <c r="E90" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="F90" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G90" s="0" t="s">
@@ -11095,7 +11107,7 @@
       <c r="E91" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="F91" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G91" s="0" t="s">
@@ -11133,7 +11145,7 @@
       <c r="E92" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F92" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G92" s="0" t="s">
@@ -11171,7 +11183,7 @@
       <c r="E93" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F93" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G93" s="0" t="s">
@@ -11209,7 +11221,7 @@
       <c r="E94" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F94" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G94" s="0" t="s">
@@ -11247,7 +11259,7 @@
       <c r="E95" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="F95" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G95" s="0" t="s">
@@ -11285,7 +11297,7 @@
       <c r="E96" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F96" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G96" s="0" t="s">
@@ -11323,7 +11335,7 @@
       <c r="E97" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="F97" s="1" t="s">
+      <c r="F97" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G97" s="0" t="s">
@@ -11361,7 +11373,7 @@
       <c r="E98" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="F98" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G98" s="0" t="s">
@@ -11399,7 +11411,7 @@
       <c r="E99" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="F99" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G99" s="0" t="s">
@@ -11437,7 +11449,7 @@
       <c r="E100" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="F100" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G100" s="0" t="s">
@@ -11475,7 +11487,7 @@
       <c r="E101" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="F101" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G101" s="0" t="s">
@@ -11513,7 +11525,7 @@
       <c r="E102" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="F102" s="1" t="s">
+      <c r="F102" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G102" s="0" t="s">
@@ -11551,7 +11563,7 @@
       <c r="E103" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="F103" s="1" t="s">
+      <c r="F103" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G103" s="0" t="s">
@@ -11589,7 +11601,7 @@
       <c r="E104" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F104" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G104" s="0" t="s">
@@ -11627,7 +11639,7 @@
       <c r="E105" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="F105" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G105" s="0" t="s">
@@ -11665,7 +11677,7 @@
       <c r="E106" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F106" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G106" s="0" t="s">
@@ -11703,7 +11715,7 @@
       <c r="E107" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="F107" s="1" t="s">
+      <c r="F107" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G107" s="0" t="s">
@@ -11741,7 +11753,7 @@
       <c r="E108" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G108" s="0" t="s">
@@ -11779,7 +11791,7 @@
       <c r="E109" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="F109" s="1" t="s">
+      <c r="F109" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G109" s="0" t="s">
@@ -11817,7 +11829,7 @@
       <c r="E110" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F110" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G110" s="0" t="s">
@@ -11855,7 +11867,7 @@
       <c r="E111" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="F111" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G111" s="0" t="s">
@@ -11893,7 +11905,7 @@
       <c r="E112" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F112" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G112" s="0" t="s">
@@ -11931,7 +11943,7 @@
       <c r="E113" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F113" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G113" s="0" t="s">
@@ -11969,7 +11981,7 @@
       <c r="E114" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F114" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G114" s="0" t="s">
@@ -12007,7 +12019,7 @@
       <c r="E115" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F115" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G115" s="0" t="s">
@@ -12045,7 +12057,7 @@
       <c r="E116" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F116" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G116" s="0" t="s">
@@ -12083,7 +12095,7 @@
       <c r="E117" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F117" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G117" s="0" t="s">
@@ -12121,7 +12133,7 @@
       <c r="E118" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F118" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G118" s="0" t="s">
@@ -12159,7 +12171,7 @@
       <c r="E119" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F119" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G119" s="0" t="s">
@@ -12197,7 +12209,7 @@
       <c r="E120" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F120" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G120" s="0" t="s">
@@ -12235,7 +12247,7 @@
       <c r="E121" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F121" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G121" s="0" t="s">
@@ -12273,7 +12285,7 @@
       <c r="E122" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F122" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G122" s="0" t="s">
@@ -12311,7 +12323,7 @@
       <c r="E123" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F123" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G123" s="0" t="s">
@@ -12349,7 +12361,7 @@
       <c r="E124" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F124" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G124" s="0" t="s">
@@ -12387,7 +12399,7 @@
       <c r="E125" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="F125" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G125" s="0" t="s">
@@ -12425,7 +12437,7 @@
       <c r="E126" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F126" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G126" s="0" t="s">
@@ -12463,7 +12475,7 @@
       <c r="E127" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="F127" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G127" s="0" t="s">
@@ -12501,7 +12513,7 @@
       <c r="E128" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F128" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G128" s="0" t="s">
@@ -12539,7 +12551,7 @@
       <c r="E129" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="F129" s="1" t="s">
+      <c r="F129" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G129" s="0" t="s">
@@ -12577,7 +12589,7 @@
       <c r="E130" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F130" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G130" s="0" t="s">
@@ -12615,7 +12627,7 @@
       <c r="E131" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F131" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G131" s="0" t="s">
@@ -12653,7 +12665,7 @@
       <c r="E132" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="F132" s="1" t="s">
+      <c r="F132" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G132" s="0" t="s">
@@ -12691,7 +12703,7 @@
       <c r="E133" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F133" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G133" s="0" t="s">
@@ -12729,7 +12741,7 @@
       <c r="E134" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F134" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G134" s="0" t="s">
@@ -12767,7 +12779,7 @@
       <c r="E135" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="F135" s="1" t="s">
+      <c r="F135" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G135" s="0" t="s">
@@ -12805,7 +12817,7 @@
       <c r="E136" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="F136" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G136" s="0" t="s">
@@ -12843,7 +12855,7 @@
       <c r="E137" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F137" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G137" s="0" t="s">
@@ -12881,7 +12893,7 @@
       <c r="E138" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="F138" s="1" t="s">
+      <c r="F138" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G138" s="0" t="s">
@@ -12919,7 +12931,7 @@
       <c r="E139" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="F139" s="1" t="s">
+      <c r="F139" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G139" s="0" t="s">
@@ -12957,7 +12969,7 @@
       <c r="E140" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="F140" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G140" s="0" t="s">
@@ -12995,7 +13007,7 @@
       <c r="E141" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="F141" s="1" t="s">
+      <c r="F141" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G141" s="0" t="s">
@@ -13033,7 +13045,7 @@
       <c r="E142" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="F142" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G142" s="0" t="s">
@@ -13071,7 +13083,7 @@
       <c r="E143" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="F143" s="1" t="s">
+      <c r="F143" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G143" s="0" t="s">
@@ -13109,7 +13121,7 @@
       <c r="E144" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="F144" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G144" s="0" t="s">
@@ -13147,7 +13159,7 @@
       <c r="E145" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="F145" s="1" t="s">
+      <c r="F145" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G145" s="0" t="s">
@@ -13185,7 +13197,7 @@
       <c r="E146" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="F146" s="1" t="s">
+      <c r="F146" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G146" s="0" t="s">
@@ -13223,7 +13235,7 @@
       <c r="E147" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F147" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G147" s="0" t="s">
@@ -13261,7 +13273,7 @@
       <c r="E148" s="0" t="s">
         <v>411</v>
       </c>
-      <c r="F148" s="1" t="s">
+      <c r="F148" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G148" s="0" t="s">
@@ -13299,7 +13311,7 @@
       <c r="E149" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="F149" s="1" t="s">
+      <c r="F149" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G149" s="0" t="s">
@@ -13337,7 +13349,7 @@
       <c r="E150" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="F150" s="1" t="s">
+      <c r="F150" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G150" s="0" t="s">
@@ -13375,7 +13387,7 @@
       <c r="E151" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="F151" s="1" t="s">
+      <c r="F151" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G151" s="0" t="s">
@@ -13413,7 +13425,7 @@
       <c r="E152" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="F152" s="1" t="s">
+      <c r="F152" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G152" s="0" t="s">
@@ -13451,7 +13463,7 @@
       <c r="E153" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="F153" s="1" t="s">
+      <c r="F153" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G153" s="0" t="s">
@@ -13489,7 +13501,7 @@
       <c r="E154" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="F154" s="1" t="s">
+      <c r="F154" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G154" s="0" t="s">
@@ -13527,7 +13539,7 @@
       <c r="E155" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="F155" s="1" t="s">
+      <c r="F155" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G155" s="0" t="s">
@@ -13565,7 +13577,7 @@
       <c r="E156" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="F156" s="1" t="s">
+      <c r="F156" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G156" s="0" t="s">
@@ -13603,7 +13615,7 @@
       <c r="E157" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="F157" s="1" t="s">
+      <c r="F157" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G157" s="0" t="s">
@@ -13641,7 +13653,7 @@
       <c r="E158" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="F158" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G158" s="0" t="s">
@@ -13679,7 +13691,7 @@
       <c r="E159" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="F159" s="1" t="s">
+      <c r="F159" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G159" s="0" t="s">
@@ -13717,7 +13729,7 @@
       <c r="E160" s="0" t="s">
         <v>442</v>
       </c>
-      <c r="F160" s="1" t="s">
+      <c r="F160" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G160" s="0" t="s">
@@ -13755,7 +13767,7 @@
       <c r="E161" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="F161" s="1" t="s">
+      <c r="F161" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G161" s="0" t="s">
@@ -13793,7 +13805,7 @@
       <c r="E162" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="F162" s="1" t="s">
+      <c r="F162" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G162" s="0" t="s">
@@ -13831,7 +13843,7 @@
       <c r="E163" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="F163" s="1" t="s">
+      <c r="F163" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G163" s="0" t="s">
@@ -13869,7 +13881,7 @@
       <c r="E164" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="F164" s="1" t="s">
+      <c r="F164" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G164" s="0" t="s">
@@ -13907,7 +13919,7 @@
       <c r="E165" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="F165" s="1" t="s">
+      <c r="F165" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G165" s="0" t="s">
@@ -13945,7 +13957,7 @@
       <c r="E166" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="F166" s="1" t="s">
+      <c r="F166" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G166" s="0" t="s">
@@ -13983,7 +13995,7 @@
       <c r="E167" s="0" t="s">
         <v>458</v>
       </c>
-      <c r="F167" s="1" t="s">
+      <c r="F167" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G167" s="0" t="s">
@@ -14021,7 +14033,7 @@
       <c r="E168" s="0" t="s">
         <v>461</v>
       </c>
-      <c r="F168" s="1" t="s">
+      <c r="F168" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G168" s="0" t="s">
@@ -14059,7 +14071,7 @@
       <c r="E169" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="F169" s="1" t="s">
+      <c r="F169" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G169" s="0" t="s">
@@ -14097,7 +14109,7 @@
       <c r="E170" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="F170" s="1" t="s">
+      <c r="F170" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G170" s="0" t="s">
@@ -14135,7 +14147,7 @@
       <c r="E171" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="F171" s="1" t="s">
+      <c r="F171" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G171" s="0" t="s">
@@ -14173,7 +14185,7 @@
       <c r="E172" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="F172" s="1" t="s">
+      <c r="F172" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G172" s="0" t="s">
@@ -14211,7 +14223,7 @@
       <c r="E173" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="F173" s="1" t="s">
+      <c r="F173" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G173" s="0" t="s">
@@ -14249,7 +14261,7 @@
       <c r="E174" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="F174" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G174" s="0" t="s">
@@ -14287,7 +14299,7 @@
       <c r="E175" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="F175" s="1" t="s">
+      <c r="F175" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G175" s="0" t="s">
@@ -14325,7 +14337,7 @@
       <c r="E176" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="F176" s="1" t="s">
+      <c r="F176" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G176" s="0" t="s">
@@ -14363,7 +14375,7 @@
       <c r="E177" s="0" t="s">
         <v>483</v>
       </c>
-      <c r="F177" s="1" t="s">
+      <c r="F177" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G177" s="0" t="s">
@@ -14401,7 +14413,7 @@
       <c r="E178" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="F178" s="1" t="s">
+      <c r="F178" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G178" s="0" t="s">
@@ -14439,7 +14451,7 @@
       <c r="E179" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="F179" s="1" t="s">
+      <c r="F179" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G179" s="0" t="s">
@@ -14477,7 +14489,7 @@
       <c r="E180" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="F180" s="1" t="s">
+      <c r="F180" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G180" s="0" t="s">
@@ -14515,7 +14527,7 @@
       <c r="E181" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="F181" s="1" t="s">
+      <c r="F181" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G181" s="0" t="s">
@@ -14553,7 +14565,7 @@
       <c r="E182" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="F182" s="1" t="s">
+      <c r="F182" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G182" s="0" t="s">
@@ -14591,7 +14603,7 @@
       <c r="E183" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="F183" s="1" t="s">
+      <c r="F183" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G183" s="0" t="s">
@@ -14629,7 +14641,7 @@
       <c r="E184" s="0" t="s">
         <v>500</v>
       </c>
-      <c r="F184" s="1" t="s">
+      <c r="F184" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G184" s="0" t="s">
@@ -14667,7 +14679,7 @@
       <c r="E185" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="F185" s="1" t="s">
+      <c r="F185" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G185" s="0" t="s">
@@ -14705,7 +14717,7 @@
       <c r="E186" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="F186" s="1" t="s">
+      <c r="F186" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G186" s="0" t="s">
@@ -14743,7 +14755,7 @@
       <c r="E187" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="F187" s="1" t="s">
+      <c r="F187" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G187" s="0" t="s">
@@ -14781,7 +14793,7 @@
       <c r="E188" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="F188" s="1" t="s">
+      <c r="F188" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G188" s="0" t="s">
@@ -14819,7 +14831,7 @@
       <c r="E189" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="F189" s="1" t="s">
+      <c r="F189" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G189" s="0" t="s">
@@ -14857,7 +14869,7 @@
       <c r="E190" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="F190" s="1" t="s">
+      <c r="F190" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G190" s="0" t="s">
@@ -14895,7 +14907,7 @@
       <c r="E191" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="F191" s="1" t="s">
+      <c r="F191" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G191" s="0" t="s">
@@ -14933,7 +14945,7 @@
       <c r="E192" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="F192" s="1" t="s">
+      <c r="F192" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G192" s="0" t="s">
@@ -14971,7 +14983,7 @@
       <c r="E193" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="F193" s="1" t="s">
+      <c r="F193" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G193" s="0" t="s">
@@ -15009,7 +15021,7 @@
       <c r="E194" s="0" t="s">
         <v>522</v>
       </c>
-      <c r="F194" s="1" t="s">
+      <c r="F194" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G194" s="0" t="s">
@@ -15047,7 +15059,7 @@
       <c r="E195" s="0" t="s">
         <v>524</v>
       </c>
-      <c r="F195" s="1" t="s">
+      <c r="F195" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G195" s="0" t="s">
@@ -15085,7 +15097,7 @@
       <c r="E196" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="F196" s="1" t="s">
+      <c r="F196" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G196" s="0" t="s">
@@ -15123,7 +15135,7 @@
       <c r="E197" s="0" t="s">
         <v>529</v>
       </c>
-      <c r="F197" s="1" t="s">
+      <c r="F197" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G197" s="0" t="s">
@@ -15161,7 +15173,7 @@
       <c r="E198" s="0" t="s">
         <v>531</v>
       </c>
-      <c r="F198" s="1" t="s">
+      <c r="F198" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G198" s="0" t="s">
@@ -15199,7 +15211,7 @@
       <c r="E199" s="0" t="s">
         <v>533</v>
       </c>
-      <c r="F199" s="1" t="s">
+      <c r="F199" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G199" s="0" t="s">
@@ -15237,7 +15249,7 @@
       <c r="E200" s="0" t="s">
         <v>535</v>
       </c>
-      <c r="F200" s="1" t="s">
+      <c r="F200" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G200" s="0" t="s">
@@ -15275,7 +15287,7 @@
       <c r="E201" s="0" t="s">
         <v>537</v>
       </c>
-      <c r="F201" s="1" t="s">
+      <c r="F201" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G201" s="0" t="s">
@@ -15313,7 +15325,7 @@
       <c r="E202" s="0" t="s">
         <v>540</v>
       </c>
-      <c r="F202" s="1" t="s">
+      <c r="F202" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G202" s="0" t="s">
@@ -15351,7 +15363,7 @@
       <c r="E203" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="F203" s="1" t="s">
+      <c r="F203" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G203" s="0" t="s">
@@ -15389,7 +15401,7 @@
       <c r="E204" s="0" t="s">
         <v>545</v>
       </c>
-      <c r="F204" s="1" t="s">
+      <c r="F204" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G204" s="0" t="s">
@@ -15427,7 +15439,7 @@
       <c r="E205" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="F205" s="1" t="s">
+      <c r="F205" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G205" s="0" t="s">
@@ -15465,7 +15477,7 @@
       <c r="E206" s="0" t="s">
         <v>550</v>
       </c>
-      <c r="F206" s="1" t="s">
+      <c r="F206" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G206" s="0" t="s">
@@ -15503,7 +15515,7 @@
       <c r="E207" s="0" t="s">
         <v>552</v>
       </c>
-      <c r="F207" s="1" t="s">
+      <c r="F207" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G207" s="0" t="s">
@@ -15541,7 +15553,7 @@
       <c r="E208" s="0" t="s">
         <v>554</v>
       </c>
-      <c r="F208" s="1" t="s">
+      <c r="F208" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G208" s="0" t="s">
@@ -15579,7 +15591,7 @@
       <c r="E209" s="0" t="s">
         <v>557</v>
       </c>
-      <c r="F209" s="1" t="s">
+      <c r="F209" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G209" s="0" t="s">
@@ -15617,7 +15629,7 @@
       <c r="E210" s="0" t="s">
         <v>560</v>
       </c>
-      <c r="F210" s="1" t="s">
+      <c r="F210" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G210" s="0" t="s">
@@ -15655,7 +15667,7 @@
       <c r="E211" s="0" t="s">
         <v>562</v>
       </c>
-      <c r="F211" s="1" t="s">
+      <c r="F211" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G211" s="0" t="s">
@@ -15693,7 +15705,7 @@
       <c r="E212" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="F212" s="1" t="s">
+      <c r="F212" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G212" s="0" t="s">
@@ -15731,7 +15743,7 @@
       <c r="E213" s="0" t="s">
         <v>567</v>
       </c>
-      <c r="F213" s="1" t="s">
+      <c r="F213" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G213" s="0" t="s">
@@ -15769,7 +15781,7 @@
       <c r="E214" s="0" t="s">
         <v>570</v>
       </c>
-      <c r="F214" s="1" t="s">
+      <c r="F214" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G214" s="0" t="s">
@@ -15807,7 +15819,7 @@
       <c r="E215" s="0" t="s">
         <v>573</v>
       </c>
-      <c r="F215" s="1" t="s">
+      <c r="F215" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G215" s="0" t="s">
@@ -15845,7 +15857,7 @@
       <c r="E216" s="0" t="s">
         <v>575</v>
       </c>
-      <c r="F216" s="1" t="s">
+      <c r="F216" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G216" s="0" t="s">
@@ -15883,7 +15895,7 @@
       <c r="E217" s="0" t="s">
         <v>578</v>
       </c>
-      <c r="F217" s="1" t="s">
+      <c r="F217" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G217" s="0" t="s">
@@ -15921,7 +15933,7 @@
       <c r="E218" s="0" t="s">
         <v>581</v>
       </c>
-      <c r="F218" s="1" t="s">
+      <c r="F218" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G218" s="0" t="s">
@@ -15959,7 +15971,7 @@
       <c r="E219" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="F219" s="1" t="s">
+      <c r="F219" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G219" s="0" t="s">
@@ -15997,7 +16009,7 @@
       <c r="E220" s="0" t="s">
         <v>586</v>
       </c>
-      <c r="F220" s="1" t="s">
+      <c r="F220" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G220" s="0" t="s">
@@ -16035,7 +16047,7 @@
       <c r="E221" s="0" t="s">
         <v>589</v>
       </c>
-      <c r="F221" s="1" t="s">
+      <c r="F221" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G221" s="0" t="s">
@@ -16073,7 +16085,7 @@
       <c r="E222" s="0" t="s">
         <v>591</v>
       </c>
-      <c r="F222" s="1" t="s">
+      <c r="F222" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G222" s="0" t="s">
@@ -16111,7 +16123,7 @@
       <c r="E223" s="0" t="s">
         <v>593</v>
       </c>
-      <c r="F223" s="1" t="s">
+      <c r="F223" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G223" s="0" t="s">
@@ -16149,7 +16161,7 @@
       <c r="E224" s="0" t="s">
         <v>595</v>
       </c>
-      <c r="F224" s="1" t="s">
+      <c r="F224" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G224" s="0" t="s">
@@ -16187,7 +16199,7 @@
       <c r="E225" s="0" t="s">
         <v>597</v>
       </c>
-      <c r="F225" s="1" t="s">
+      <c r="F225" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G225" s="0" t="s">
@@ -16225,7 +16237,7 @@
       <c r="E226" s="0" t="s">
         <v>599</v>
       </c>
-      <c r="F226" s="1" t="s">
+      <c r="F226" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G226" s="0" t="s">
@@ -16263,7 +16275,7 @@
       <c r="E227" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="F227" s="1" t="s">
+      <c r="F227" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G227" s="0" t="s">
@@ -16301,7 +16313,7 @@
       <c r="E228" s="0" t="s">
         <v>604</v>
       </c>
-      <c r="F228" s="1" t="s">
+      <c r="F228" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G228" s="0" t="s">
@@ -16339,7 +16351,7 @@
       <c r="E229" s="0" t="s">
         <v>607</v>
       </c>
-      <c r="F229" s="1" t="s">
+      <c r="F229" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G229" s="0" t="s">
@@ -16377,7 +16389,7 @@
       <c r="E230" s="0" t="s">
         <v>609</v>
       </c>
-      <c r="F230" s="1" t="s">
+      <c r="F230" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G230" s="0" t="s">
@@ -16415,7 +16427,7 @@
       <c r="E231" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="F231" s="1" t="s">
+      <c r="F231" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G231" s="0" t="s">
@@ -16453,7 +16465,7 @@
       <c r="E232" s="0" t="s">
         <v>614</v>
       </c>
-      <c r="F232" s="1" t="s">
+      <c r="F232" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G232" s="0" t="s">
@@ -16491,7 +16503,7 @@
       <c r="E233" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="F233" s="1" t="s">
+      <c r="F233" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G233" s="0" t="s">
@@ -16529,7 +16541,7 @@
       <c r="E234" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="F234" s="1" t="s">
+      <c r="F234" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G234" s="0" t="s">
@@ -16567,7 +16579,7 @@
       <c r="E235" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="F235" s="1" t="s">
+      <c r="F235" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G235" s="0" t="s">
@@ -16605,7 +16617,7 @@
       <c r="E236" s="0" t="s">
         <v>625</v>
       </c>
-      <c r="F236" s="1" t="s">
+      <c r="F236" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G236" s="0" t="s">
@@ -16643,7 +16655,7 @@
       <c r="E237" s="0" t="s">
         <v>628</v>
       </c>
-      <c r="F237" s="1" t="s">
+      <c r="F237" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G237" s="0" t="s">
@@ -16681,7 +16693,7 @@
       <c r="E238" s="0" t="s">
         <v>631</v>
       </c>
-      <c r="F238" s="1" t="s">
+      <c r="F238" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G238" s="0" t="s">
@@ -16719,7 +16731,7 @@
       <c r="E239" s="0" t="s">
         <v>633</v>
       </c>
-      <c r="F239" s="1" t="s">
+      <c r="F239" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G239" s="0" t="s">
@@ -16757,7 +16769,7 @@
       <c r="E240" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="F240" s="1" t="s">
+      <c r="F240" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G240" s="0" t="s">
@@ -16795,7 +16807,7 @@
       <c r="E241" s="0" t="s">
         <v>641</v>
       </c>
-      <c r="F241" s="1" t="s">
+      <c r="F241" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G241" s="0" t="s">
@@ -16833,7 +16845,7 @@
       <c r="E242" s="0" t="s">
         <v>644</v>
       </c>
-      <c r="F242" s="1" t="s">
+      <c r="F242" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G242" s="0" t="s">
@@ -16871,7 +16883,7 @@
       <c r="E243" s="0" t="s">
         <v>646</v>
       </c>
-      <c r="F243" s="1" t="s">
+      <c r="F243" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G243" s="0" t="s">
@@ -16909,7 +16921,7 @@
       <c r="E244" s="0" t="s">
         <v>649</v>
       </c>
-      <c r="F244" s="1" t="s">
+      <c r="F244" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G244" s="0" t="s">
@@ -16947,7 +16959,7 @@
       <c r="E245" s="0" t="s">
         <v>651</v>
       </c>
-      <c r="F245" s="1" t="s">
+      <c r="F245" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G245" s="0" t="s">
@@ -16985,7 +16997,7 @@
       <c r="E246" s="0" t="s">
         <v>654</v>
       </c>
-      <c r="F246" s="1" t="s">
+      <c r="F246" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G246" s="0" t="s">
@@ -17023,7 +17035,7 @@
       <c r="E247" s="0" t="s">
         <v>657</v>
       </c>
-      <c r="F247" s="1" t="s">
+      <c r="F247" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G247" s="0" t="s">
@@ -17061,7 +17073,7 @@
       <c r="E248" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="F248" s="1" t="s">
+      <c r="F248" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G248" s="0" t="s">
@@ -17099,7 +17111,7 @@
       <c r="E249" s="0" t="s">
         <v>663</v>
       </c>
-      <c r="F249" s="1" t="s">
+      <c r="F249" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G249" s="0" t="s">
@@ -17137,7 +17149,7 @@
       <c r="E250" s="0" t="s">
         <v>666</v>
       </c>
-      <c r="F250" s="1" t="s">
+      <c r="F250" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G250" s="0" t="s">
@@ -17175,7 +17187,7 @@
       <c r="E251" s="0" t="s">
         <v>669</v>
       </c>
-      <c r="F251" s="1" t="s">
+      <c r="F251" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G251" s="0" t="s">
@@ -17213,7 +17225,7 @@
       <c r="E252" s="0" t="s">
         <v>673</v>
       </c>
-      <c r="F252" s="1" t="s">
+      <c r="F252" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G252" s="0" t="s">
@@ -17251,7 +17263,7 @@
       <c r="E253" s="0" t="s">
         <v>676</v>
       </c>
-      <c r="F253" s="1" t="s">
+      <c r="F253" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G253" s="0" t="s">
@@ -17289,7 +17301,7 @@
       <c r="E254" s="0" t="s">
         <v>679</v>
       </c>
-      <c r="F254" s="1" t="s">
+      <c r="F254" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G254" s="0" t="s">
@@ -17327,7 +17339,7 @@
       <c r="E255" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="F255" s="1" t="s">
+      <c r="F255" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G255" s="0" t="s">
@@ -17365,7 +17377,7 @@
       <c r="E256" s="0" t="s">
         <v>684</v>
       </c>
-      <c r="F256" s="1" t="s">
+      <c r="F256" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G256" s="0" t="s">
@@ -17403,7 +17415,7 @@
       <c r="E257" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="F257" s="1" t="s">
+      <c r="F257" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G257" s="0" t="s">
@@ -17441,7 +17453,7 @@
       <c r="E258" s="0" t="s">
         <v>691</v>
       </c>
-      <c r="F258" s="1" t="s">
+      <c r="F258" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G258" s="0" t="s">
@@ -17479,7 +17491,7 @@
       <c r="E259" s="0" t="s">
         <v>695</v>
       </c>
-      <c r="F259" s="1" t="s">
+      <c r="F259" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G259" s="0" t="s">
@@ -17517,7 +17529,7 @@
       <c r="E260" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="F260" s="1" t="s">
+      <c r="F260" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G260" s="0" t="s">
@@ -17555,7 +17567,7 @@
       <c r="E261" s="0" t="s">
         <v>702</v>
       </c>
-      <c r="F261" s="1" t="s">
+      <c r="F261" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G261" s="0" t="s">
@@ -17593,7 +17605,7 @@
       <c r="E262" s="0" t="s">
         <v>705</v>
       </c>
-      <c r="F262" s="1" t="s">
+      <c r="F262" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G262" s="0" t="s">
@@ -17631,7 +17643,7 @@
       <c r="E263" s="0" t="s">
         <v>707</v>
       </c>
-      <c r="F263" s="1" t="s">
+      <c r="F263" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G263" s="0" t="s">
@@ -17669,7 +17681,7 @@
       <c r="E264" s="0" t="s">
         <v>709</v>
       </c>
-      <c r="F264" s="1" t="s">
+      <c r="F264" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G264" s="0" t="s">
@@ -17707,7 +17719,7 @@
       <c r="E265" s="0" t="s">
         <v>712</v>
       </c>
-      <c r="F265" s="1" t="s">
+      <c r="F265" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G265" s="0" t="s">
@@ -17745,7 +17757,7 @@
       <c r="E266" s="0" t="s">
         <v>715</v>
       </c>
-      <c r="F266" s="1" t="s">
+      <c r="F266" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G266" s="0" t="s">
@@ -17783,7 +17795,7 @@
       <c r="E267" s="0" t="s">
         <v>718</v>
       </c>
-      <c r="F267" s="1" t="s">
+      <c r="F267" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G267" s="0" t="s">
@@ -17821,7 +17833,7 @@
       <c r="E268" s="0" t="s">
         <v>720</v>
       </c>
-      <c r="F268" s="1" t="s">
+      <c r="F268" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G268" s="0" t="s">
@@ -17859,7 +17871,7 @@
       <c r="E269" s="0" t="s">
         <v>723</v>
       </c>
-      <c r="F269" s="1" t="s">
+      <c r="F269" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G269" s="0" t="s">
@@ -17897,7 +17909,7 @@
       <c r="E270" s="0" t="s">
         <v>726</v>
       </c>
-      <c r="F270" s="1" t="s">
+      <c r="F270" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G270" s="0" t="s">
@@ -17935,7 +17947,7 @@
       <c r="E271" s="0" t="s">
         <v>729</v>
       </c>
-      <c r="F271" s="1" t="s">
+      <c r="F271" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G271" s="0" t="s">
@@ -17973,7 +17985,7 @@
       <c r="E272" s="0" t="s">
         <v>732</v>
       </c>
-      <c r="F272" s="1" t="s">
+      <c r="F272" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G272" s="0" t="s">
@@ -18011,7 +18023,7 @@
       <c r="E273" s="0" t="s">
         <v>735</v>
       </c>
-      <c r="F273" s="1" t="s">
+      <c r="F273" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G273" s="0" t="s">
@@ -18049,7 +18061,7 @@
       <c r="E274" s="0" t="s">
         <v>738</v>
       </c>
-      <c r="F274" s="1" t="s">
+      <c r="F274" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G274" s="0" t="s">
@@ -18087,7 +18099,7 @@
       <c r="E275" s="0" t="s">
         <v>741</v>
       </c>
-      <c r="F275" s="1" t="s">
+      <c r="F275" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G275" s="0" t="s">
@@ -18125,7 +18137,7 @@
       <c r="E276" s="0" t="s">
         <v>744</v>
       </c>
-      <c r="F276" s="1" t="s">
+      <c r="F276" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G276" s="0" t="s">
@@ -18163,7 +18175,7 @@
       <c r="E277" s="0" t="s">
         <v>746</v>
       </c>
-      <c r="F277" s="1" t="s">
+      <c r="F277" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G277" s="0" t="s">
@@ -18201,7 +18213,7 @@
       <c r="E278" s="0" t="s">
         <v>749</v>
       </c>
-      <c r="F278" s="1" t="s">
+      <c r="F278" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G278" s="0" t="s">
@@ -18239,7 +18251,7 @@
       <c r="E279" s="0" t="s">
         <v>752</v>
       </c>
-      <c r="F279" s="1" t="s">
+      <c r="F279" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G279" s="0" t="s">
@@ -18277,7 +18289,7 @@
       <c r="E280" s="0" t="s">
         <v>755</v>
       </c>
-      <c r="F280" s="1" t="s">
+      <c r="F280" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G280" s="0" t="s">
@@ -18315,7 +18327,7 @@
       <c r="E281" s="0" t="s">
         <v>757</v>
       </c>
-      <c r="F281" s="1" t="s">
+      <c r="F281" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G281" s="0" t="s">
@@ -18353,7 +18365,7 @@
       <c r="E282" s="0" t="s">
         <v>760</v>
       </c>
-      <c r="F282" s="1" t="s">
+      <c r="F282" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G282" s="0" t="s">
@@ -18391,7 +18403,7 @@
       <c r="E283" s="0" t="s">
         <v>762</v>
       </c>
-      <c r="F283" s="1" t="s">
+      <c r="F283" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G283" s="0" t="s">
@@ -18429,7 +18441,7 @@
       <c r="E284" s="0" t="s">
         <v>765</v>
       </c>
-      <c r="F284" s="1" t="s">
+      <c r="F284" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G284" s="0" t="s">
@@ -18467,7 +18479,7 @@
       <c r="E285" s="0" t="s">
         <v>768</v>
       </c>
-      <c r="F285" s="1" t="s">
+      <c r="F285" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G285" s="0" t="s">
@@ -18505,7 +18517,7 @@
       <c r="E286" s="0" t="s">
         <v>771</v>
       </c>
-      <c r="F286" s="1" t="s">
+      <c r="F286" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G286" s="0" t="s">
@@ -18543,7 +18555,7 @@
       <c r="E287" s="0" t="s">
         <v>774</v>
       </c>
-      <c r="F287" s="1" t="s">
+      <c r="F287" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G287" s="0" t="s">
@@ -18581,7 +18593,7 @@
       <c r="E288" s="0" t="s">
         <v>777</v>
       </c>
-      <c r="F288" s="1" t="s">
+      <c r="F288" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G288" s="0" t="s">
@@ -18619,7 +18631,7 @@
       <c r="E289" s="0" t="s">
         <v>780</v>
       </c>
-      <c r="F289" s="1" t="s">
+      <c r="F289" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G289" s="0" t="s">
@@ -18657,7 +18669,7 @@
       <c r="E290" s="0" t="s">
         <v>783</v>
       </c>
-      <c r="F290" s="1" t="s">
+      <c r="F290" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G290" s="0" t="s">
@@ -18695,7 +18707,7 @@
       <c r="E291" s="0" t="s">
         <v>786</v>
       </c>
-      <c r="F291" s="1" t="s">
+      <c r="F291" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G291" s="0" t="s">
@@ -18733,7 +18745,7 @@
       <c r="E292" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="F292" s="1" t="s">
+      <c r="F292" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G292" s="0" t="s">
@@ -18771,7 +18783,7 @@
       <c r="E293" s="0" t="s">
         <v>792</v>
       </c>
-      <c r="F293" s="1" t="s">
+      <c r="F293" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G293" s="0" t="s">
@@ -18809,7 +18821,7 @@
       <c r="E294" s="0" t="s">
         <v>795</v>
       </c>
-      <c r="F294" s="1" t="s">
+      <c r="F294" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G294" s="0" t="s">
@@ -18847,7 +18859,7 @@
       <c r="E295" s="0" t="s">
         <v>798</v>
       </c>
-      <c r="F295" s="1" t="s">
+      <c r="F295" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G295" s="0" t="s">
@@ -18885,7 +18897,7 @@
       <c r="E296" s="0" t="s">
         <v>801</v>
       </c>
-      <c r="F296" s="1" t="s">
+      <c r="F296" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G296" s="0" t="s">
@@ -35301,7 +35313,7 @@
       <c r="E728" s="0" t="s">
         <v>595</v>
       </c>
-      <c r="F728" s="1" t="s">
+      <c r="F728" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G728" s="0" t="s">
@@ -35339,7 +35351,7 @@
       <c r="E729" s="0" t="s">
         <v>597</v>
       </c>
-      <c r="F729" s="1" t="s">
+      <c r="F729" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G729" s="0" t="s">
@@ -35377,7 +35389,7 @@
       <c r="E730" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="F730" s="1" t="s">
+      <c r="F730" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G730" s="0" t="s">
@@ -35415,7 +35427,7 @@
       <c r="E731" s="0" t="s">
         <v>2243</v>
       </c>
-      <c r="F731" s="1" t="s">
+      <c r="F731" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G731" s="0" t="s">
@@ -35453,7 +35465,7 @@
       <c r="E732" s="0" t="s">
         <v>1931</v>
       </c>
-      <c r="F732" s="1" t="s">
+      <c r="F732" s="2" t="s">
         <v>692</v>
       </c>
       <c r="G732" s="0" t="s">
@@ -35491,7 +35503,7 @@
       <c r="E733" s="0" t="s">
         <v>2087</v>
       </c>
-      <c r="F733" s="1" t="s">
+      <c r="F733" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G733" s="0" t="s">
@@ -35529,7 +35541,7 @@
       <c r="E734" s="0" t="s">
         <v>2248</v>
       </c>
-      <c r="F734" s="1" t="s">
+      <c r="F734" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G734" s="0" t="s">
@@ -35567,7 +35579,7 @@
       <c r="E735" s="0" t="s">
         <v>2251</v>
       </c>
-      <c r="F735" s="1" t="s">
+      <c r="F735" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G735" s="0" t="s">
@@ -35605,7 +35617,7 @@
       <c r="E736" s="0" t="s">
         <v>2253</v>
       </c>
-      <c r="F736" s="1" t="s">
+      <c r="F736" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G736" s="0" t="s">
@@ -35643,7 +35655,7 @@
       <c r="E737" s="0" t="s">
         <v>2255</v>
       </c>
-      <c r="F737" s="1" t="s">
+      <c r="F737" s="2" t="s">
         <v>699</v>
       </c>
       <c r="G737" s="0" t="s">
@@ -35681,7 +35693,7 @@
       <c r="E738" s="0" t="s">
         <v>2258</v>
       </c>
-      <c r="F738" s="1" t="s">
+      <c r="F738" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G738" s="0" t="s">
@@ -35719,7 +35731,7 @@
       <c r="E739" s="0" t="s">
         <v>2262</v>
       </c>
-      <c r="F739" s="1" t="s">
+      <c r="F739" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G739" s="0" t="s">
@@ -35757,7 +35769,7 @@
       <c r="E740" s="0" t="s">
         <v>2265</v>
       </c>
-      <c r="F740" s="1" t="s">
+      <c r="F740" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G740" s="0" t="s">
@@ -35795,7 +35807,7 @@
       <c r="E741" s="0" t="s">
         <v>2267</v>
       </c>
-      <c r="F741" s="1" t="s">
+      <c r="F741" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G741" s="0" t="s">
@@ -35833,7 +35845,7 @@
       <c r="E742" s="0" t="s">
         <v>2269</v>
       </c>
-      <c r="F742" s="1" t="s">
+      <c r="F742" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G742" s="0" t="s">
@@ -35871,7 +35883,7 @@
       <c r="E743" s="0" t="s">
         <v>2271</v>
       </c>
-      <c r="F743" s="1" t="s">
+      <c r="F743" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G743" s="0" t="s">
@@ -35909,7 +35921,7 @@
       <c r="E744" s="0" t="s">
         <v>2273</v>
       </c>
-      <c r="F744" s="1" t="s">
+      <c r="F744" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G744" s="0" t="s">
@@ -35947,7 +35959,7 @@
       <c r="E745" s="0" t="s">
         <v>2276</v>
       </c>
-      <c r="F745" s="1" t="s">
+      <c r="F745" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G745" s="0" t="s">
@@ -35985,7 +35997,7 @@
       <c r="E746" s="0" t="s">
         <v>2279</v>
       </c>
-      <c r="F746" s="1" t="s">
+      <c r="F746" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G746" s="0" t="s">
@@ -36023,7 +36035,7 @@
       <c r="E747" s="0" t="s">
         <v>2282</v>
       </c>
-      <c r="F747" s="1" t="s">
+      <c r="F747" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G747" s="0" t="s">
@@ -36061,7 +36073,7 @@
       <c r="E748" s="0" t="s">
         <v>2284</v>
       </c>
-      <c r="F748" s="1" t="s">
+      <c r="F748" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G748" s="0" t="s">
@@ -36099,7 +36111,7 @@
       <c r="E749" s="0" t="s">
         <v>2287</v>
       </c>
-      <c r="F749" s="1" t="s">
+      <c r="F749" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G749" s="0" t="s">
@@ -36137,7 +36149,7 @@
       <c r="E750" s="0" t="s">
         <v>2289</v>
       </c>
-      <c r="F750" s="1" t="s">
+      <c r="F750" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G750" s="0" t="s">

</xml_diff>